<commit_message>
RMarkdwon file added with a plot
</commit_message>
<xml_diff>
--- a/raw_data/data.xlsx
+++ b/raw_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25db413838a0c1ce/1. PhD GU/1. Research/github_test_repo/test_repo/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16A1A50F-0BD7-40C1-B7C7-12F884218EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{16A1A50F-0BD7-40C1-B7C7-12F884218EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{754C2945-16D7-41DB-A17E-397D008752F8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2070" windowWidth="21600" windowHeight="11265" xr2:uid="{A2F75634-BE6A-4F7A-84B2-4FADCC9F97E9}"/>
   </bookViews>
@@ -410,13 +410,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D4D9AE-6B1B-485D-94BA-6A83C3A28C2D}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
@@ -442,6 +443,10 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,C2,D2,A2)</f>
+        <v>0_sacculus_1</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>
@@ -456,6 +461,10 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B41" si="0">_xlfn.TEXTJOIN("_",TRUE,C3,D3,A3)</f>
+        <v>0_sacculus_2</v>
+      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -470,6 +479,10 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>0_sacculus_3</v>
+      </c>
       <c r="C4">
         <v>0</v>
       </c>
@@ -484,6 +497,10 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>0_sacculus_4</v>
+      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -498,6 +515,10 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>0_sacculus_5</v>
+      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -511,6 +532,10 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>0_acuminata_6</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -526,6 +551,10 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>0_acuminata_7</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -540,6 +569,10 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>0_acuminata_8</v>
+      </c>
       <c r="C9">
         <v>0</v>
       </c>
@@ -554,6 +587,10 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>0_acuminata_9</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
@@ -568,6 +605,10 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>0_acuminata_10</v>
+      </c>
       <c r="C11">
         <v>0</v>
       </c>
@@ -582,6 +623,10 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>1_sacculus_11</v>
+      </c>
       <c r="C12">
         <v>1</v>
       </c>
@@ -596,6 +641,10 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>1_sacculus_12</v>
+      </c>
       <c r="C13">
         <v>1</v>
       </c>
@@ -610,6 +659,10 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>1_sacculus_13</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -624,6 +677,10 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>1_sacculus_14</v>
+      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -638,6 +695,10 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>1_sacculus_15</v>
+      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -652,6 +713,10 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>1_acuminata_16</v>
+      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -666,6 +731,10 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>1_acuminata_17</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -680,6 +749,10 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>1_acuminata_18</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -694,6 +767,10 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>1_acuminata_19</v>
+      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -708,6 +785,10 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>1_acuminata_20</v>
+      </c>
       <c r="C21">
         <v>1</v>
       </c>
@@ -722,6 +803,10 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>2_sacculus_21</v>
+      </c>
       <c r="C22">
         <v>2</v>
       </c>
@@ -736,6 +821,10 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>2_sacculus_22</v>
+      </c>
       <c r="C23">
         <v>2</v>
       </c>
@@ -750,6 +839,10 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>2_sacculus_23</v>
+      </c>
       <c r="C24">
         <v>2</v>
       </c>
@@ -764,6 +857,10 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>2_sacculus_24</v>
+      </c>
       <c r="C25">
         <v>2</v>
       </c>
@@ -778,6 +875,10 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>2_sacculus_25</v>
+      </c>
       <c r="C26">
         <v>2</v>
       </c>
@@ -792,6 +893,10 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>2_acuminata_26</v>
+      </c>
       <c r="C27">
         <v>2</v>
       </c>
@@ -806,6 +911,10 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>2_acuminata_27</v>
+      </c>
       <c r="C28">
         <v>2</v>
       </c>
@@ -820,6 +929,10 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>2_acuminata_28</v>
+      </c>
       <c r="C29">
         <v>2</v>
       </c>
@@ -834,6 +947,10 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>2_acuminata_29</v>
+      </c>
       <c r="C30">
         <v>2</v>
       </c>
@@ -848,6 +965,10 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>2_acuminata_30</v>
+      </c>
       <c r="C31">
         <v>2</v>
       </c>
@@ -862,6 +983,10 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>5_sacculus_31</v>
+      </c>
       <c r="C32">
         <v>5</v>
       </c>
@@ -876,6 +1001,10 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>5_sacculus_32</v>
+      </c>
       <c r="C33">
         <v>5</v>
       </c>
@@ -890,6 +1019,10 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>5_sacculus_33</v>
+      </c>
       <c r="C34">
         <v>5</v>
       </c>
@@ -904,6 +1037,10 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>5_sacculus_34</v>
+      </c>
       <c r="C35">
         <v>5</v>
       </c>
@@ -918,6 +1055,10 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>5_sacculus_35</v>
+      </c>
       <c r="C36">
         <v>5</v>
       </c>
@@ -932,6 +1073,10 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>5_acuminata_36</v>
+      </c>
       <c r="C37">
         <v>5</v>
       </c>
@@ -946,6 +1091,10 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>5_acuminata_37</v>
+      </c>
       <c r="C38">
         <v>5</v>
       </c>
@@ -960,6 +1109,10 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>5_acuminata_38</v>
+      </c>
       <c r="C39">
         <v>5</v>
       </c>
@@ -974,6 +1127,10 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>5_acuminata_39</v>
+      </c>
       <c r="C40">
         <v>5</v>
       </c>
@@ -987,6 +1144,10 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>5_acuminata_40</v>
       </c>
       <c r="C41">
         <v>5</v>

</xml_diff>